<commit_message>
Atualização do arquivo de docs recebidos
</commit_message>
<xml_diff>
--- a/03_contDocsRecebidos.xlsx
+++ b/03_contDocsRecebidos.xlsx
@@ -721,13 +721,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BE584F2-A51E-4494-B8A6-5D96512C55B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C88F0074-7568-4A4C-AC11-968D7BA65CB6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6863545-E295-4C91-AFA5-9CBD31007952}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{211B57C0-3CE0-41AD-9CE2-364DA9CC13B9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C2E58D6-4B01-4DDB-8B68-F8505476BFDD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F446BEFA-529A-4331-96A1-FCDDC495C816}"/>
 </file>
</xml_diff>